<commit_message>
Multiple Equal Poles 8
</commit_message>
<xml_diff>
--- a/Benchmark_System/Multiple Equal Poles 8/Multiple Equal Poles8_dist.xlsx
+++ b/Benchmark_System/Multiple Equal Poles 8/Multiple Equal Poles8_dist.xlsx
@@ -138,10 +138,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4.9383684503676211</v>
+        <v>4.9372844376893701</v>
       </c>
       <c r="C2">
-        <v>2.0735280324958567</v>
+        <v>2.0588463868717524</v>
       </c>
     </row>
     <row r="3">
@@ -149,10 +149,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.1556958468426242</v>
+        <v>1.1558967911587537</v>
       </c>
       <c r="C3">
-        <v>3.2996999356239827</v>
+        <v>3.2852655384412373</v>
       </c>
     </row>
     <row r="4">
@@ -160,10 +160,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.321292279377646</v>
+        <v>4.3201072330525276</v>
       </c>
       <c r="C4">
-        <v>5.3262966820907964</v>
+        <v>5.2624351432080676</v>
       </c>
     </row>
     <row r="5">
@@ -171,10 +171,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.886291980287135</v>
+        <v>2.8874878263154731</v>
       </c>
       <c r="C5">
-        <v>2.9908047585257158</v>
+        <v>3.0522904438843694</v>
       </c>
     </row>
     <row r="6">
@@ -182,7 +182,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>5.4887571611286781</v>
+        <v>5.5522896573485676</v>
       </c>
     </row>
     <row r="7">
@@ -212,10 +212,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>106.7292493876007</v>
+        <v>109.43629248616479</v>
       </c>
       <c r="C9">
-        <v>2.3166353423612946</v>
+        <v>2.3418180302461367</v>
       </c>
     </row>
     <row r="10">
@@ -223,7 +223,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>139.62251985721954</v>
+        <v>154.60363398197694</v>
       </c>
     </row>
     <row r="11">
@@ -242,10 +242,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>36.689692823134131</v>
+        <v>36.684652282188203</v>
       </c>
       <c r="C12">
-        <v>32.364100217053213</v>
+        <v>32.237774215338959</v>
       </c>
     </row>
     <row r="13">
@@ -275,10 +275,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.5984631223015987</v>
+        <v>0.59834630534917566</v>
       </c>
       <c r="C15">
-        <v>0.35461464345652605</v>
+        <v>0.35330435208717326</v>
       </c>
     </row>
     <row r="16">
@@ -286,10 +286,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10.01242034107373</v>
+        <v>10.012651951040695</v>
       </c>
       <c r="C16">
-        <v>8.0892802715341467</v>
+        <v>8.0539692291398843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>